<commit_message>
Added snapshots + update README
</commit_message>
<xml_diff>
--- a/christmas_geekster_2022/christmas_movies_dataset.xlsx
+++ b/christmas_geekster_2022/christmas_movies_dataset.xlsx
@@ -30085,4 +30085,10 @@
     <ignoredError sqref="A2:D37 B1 F1 E2:I37 H1 J1 J2:K37 L2:V37 A279:D279 E279:I279 J279:K279 L279:V279 A278:D278 E278:I278 J278:K278 L278:V278 A271:D277 E271:I277 J271:K277 L271:V277 A269:D270 E269:I270 J269:K270 L269:V270 A264:D268 E264:I268 J264:K268 L264:V268 A259:D263 E259:I263 J259:K263 L259:V263 A38:D258 E38:I258 J38:K258 L38:V258" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>